<commit_message>
Update db for Product
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uithcm-my.sharepoint.com/personal/21520442_ms_uit_edu_vn/Documents/HKV/Internet &amp; Công nghệ web/FurnitureWebsite/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="540" documentId="14_{7FF668E4-114F-45F3-93BD-413DF14B2BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D08CC9D-1D9B-4FC9-92D6-208240612EA4}"/>
+  <xr:revisionPtr revIDLastSave="547" documentId="14_{7FF668E4-114F-45F3-93BD-413DF14B2BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFD18C67-CF38-4B93-82A1-7B3DBED5C7B1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EDD4E223-FED4-45DA-A9CC-BEB910C23BCF}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="224">
   <si>
     <t>Bedroom</t>
   </si>
@@ -439,114 +439,12 @@
     <t>Barcode</t>
   </si>
   <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Yellow</t>
-  </si>
-  <si>
-    <t>Purple</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>Pink</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
     <t>White</t>
   </si>
   <si>
-    <t>#FF0000</t>
-  </si>
-  <si>
-    <t>#00FF00</t>
-  </si>
-  <si>
-    <t>#0000FF</t>
-  </si>
-  <si>
-    <t>#FFFF00</t>
-  </si>
-  <si>
-    <t>#800080</t>
-  </si>
-  <si>
-    <t>#FFA500</t>
-  </si>
-  <si>
-    <t>#FFC0CB</t>
-  </si>
-  <si>
-    <t>#A52A2A</t>
-  </si>
-  <si>
-    <t>#000000</t>
-  </si>
-  <si>
     <t>#FFFFFF</t>
   </si>
   <si>
-    <t>Mahogany</t>
-  </si>
-  <si>
-    <t>#420D09</t>
-  </si>
-  <si>
-    <t>Walnut</t>
-  </si>
-  <si>
-    <t>#5E483E</t>
-  </si>
-  <si>
-    <t>Oak</t>
-  </si>
-  <si>
-    <t>#8B735B</t>
-  </si>
-  <si>
-    <t>Cherry</t>
-  </si>
-  <si>
-    <t>#B23B00</t>
-  </si>
-  <si>
-    <t>Espresso</t>
-  </si>
-  <si>
-    <t>#4F2A1D</t>
-  </si>
-  <si>
-    <t>Maple</t>
-  </si>
-  <si>
-    <t>#C68E55</t>
-  </si>
-  <si>
-    <t>Ebony</t>
-  </si>
-  <si>
-    <t>#555D61</t>
-  </si>
-  <si>
-    <t>Chestnut</t>
-  </si>
-  <si>
-    <t>#954E2A</t>
-  </si>
-  <si>
     <t>Ash</t>
   </si>
   <si>
@@ -668,6 +566,156 @@
   </si>
   <si>
     <t>A fresh update on a beloved classic. The Carmine’s fan-pleated arms bring it understated elegance. The tailored seat and back offer a supportive sit.</t>
+  </si>
+  <si>
+    <t>ImgDirect</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\1</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\2</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\3</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\4</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\5</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\6</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\7</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\8</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\9</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\10</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\11</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\12</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\13</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\14</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\15</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\16</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\17</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\18</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\19</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\20</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\21</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\22</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\23</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\24</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\25</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\26</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\27</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\28</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\29</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\30</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\31</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\32</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\33</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\34</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\35</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\36</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\37</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\38</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\39</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\40</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\41</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\42</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\43</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\44</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\45</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\46</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\47</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\48</t>
+  </si>
+  <si>
+    <t>\img\Products_Photos\49</t>
   </si>
 </sst>
 </file>
@@ -1055,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4AED73-D74A-4FB9-9481-FBDC8FFD72A2}">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1067,10 +1115,12 @@
     <col min="2" max="2" width="32.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="10.42578125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1098,8 +1148,11 @@
       <c r="I1" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1127,8 +1180,11 @@
       <c r="I2" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1156,8 +1212,11 @@
       <c r="I3" s="1">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1185,8 +1244,11 @@
       <c r="I4" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1194,7 +1256,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
       <c r="D5" s="1">
         <v>2475</v>
@@ -1214,8 +1276,11 @@
       <c r="I5" s="1">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1223,7 +1288,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
       <c r="D6" s="1">
         <v>1950</v>
@@ -1243,8 +1308,11 @@
       <c r="I6" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1272,8 +1340,11 @@
       <c r="I7" s="1">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1301,8 +1372,11 @@
       <c r="I8" s="1">
         <v>82</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1330,8 +1404,11 @@
       <c r="I9" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1359,8 +1436,11 @@
       <c r="I10" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1388,8 +1468,11 @@
       <c r="I11" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1417,8 +1500,11 @@
       <c r="I12" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1446,8 +1532,11 @@
       <c r="I13" s="1">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1475,8 +1564,11 @@
       <c r="I14" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1504,8 +1596,11 @@
       <c r="I15" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1533,8 +1628,11 @@
       <c r="I16" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1562,8 +1660,11 @@
       <c r="I17" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1591,8 +1692,11 @@
       <c r="I18" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1620,8 +1724,11 @@
       <c r="I19" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1649,8 +1756,11 @@
       <c r="I20" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1678,8 +1788,11 @@
       <c r="I21" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1707,8 +1820,11 @@
       <c r="I22" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1736,8 +1852,11 @@
       <c r="I23" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1765,8 +1884,11 @@
       <c r="I24" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1794,8 +1916,11 @@
       <c r="I25" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1823,8 +1948,11 @@
       <c r="I26" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1852,8 +1980,11 @@
       <c r="I27" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1881,8 +2012,11 @@
       <c r="I28" s="1">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1910,8 +2044,11 @@
       <c r="I29" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1939,8 +2076,11 @@
       <c r="I30" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1968,8 +2108,11 @@
       <c r="I31" s="1">
         <v>19.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1977,7 +2120,7 @@
         <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
       <c r="D32" s="1">
         <v>2450</v>
@@ -1997,8 +2140,11 @@
       <c r="I32" s="1">
         <v>96</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2026,8 +2172,11 @@
       <c r="I33" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2035,7 +2184,7 @@
         <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>204</v>
+        <v>170</v>
       </c>
       <c r="D34" s="1">
         <v>755</v>
@@ -2055,8 +2204,11 @@
       <c r="I34" s="1">
         <v>19.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2064,7 +2216,7 @@
         <v>46</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
       <c r="D35" s="1">
         <v>4275</v>
@@ -2084,8 +2236,11 @@
       <c r="I35" s="1">
         <v>96</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2093,7 +2248,7 @@
         <v>47</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>205</v>
+        <v>171</v>
       </c>
       <c r="D36" s="1">
         <v>2925</v>
@@ -2113,8 +2268,11 @@
       <c r="I36" s="1">
         <v>48</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2122,7 +2280,7 @@
         <v>48</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="D37" s="1">
         <v>525</v>
@@ -2142,8 +2300,11 @@
       <c r="I37" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2171,8 +2332,11 @@
       <c r="I38" s="1">
         <v>43</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2200,8 +2364,11 @@
       <c r="I39" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2209,7 +2376,7 @@
         <v>50</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="D40" s="1">
         <v>4250</v>
@@ -2229,8 +2396,11 @@
       <c r="I40" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2258,8 +2428,11 @@
       <c r="I41" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2287,8 +2460,11 @@
       <c r="I42" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2316,8 +2492,11 @@
       <c r="I43" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2345,8 +2524,11 @@
       <c r="I44" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2374,8 +2556,11 @@
       <c r="I45" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2403,8 +2588,11 @@
       <c r="I46" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2432,8 +2620,11 @@
       <c r="I47" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2461,8 +2652,11 @@
       <c r="I48" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2490,8 +2684,11 @@
       <c r="I49" s="1">
         <v>58</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2519,8 +2716,12 @@
       <c r="I50" s="1">
         <v>100</v>
       </c>
+      <c r="J50" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3623,10 +3824,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9883094F-7846-469A-A05E-E54F036B4DF3}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3650,7 +3851,7 @@
         <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3658,10 +3859,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3669,197 +3870,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
         <v>136</v>
-      </c>
-      <c r="C7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>138</v>
-      </c>
-      <c r="C9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>153</v>
-      </c>
-      <c r="C13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>157</v>
-      </c>
-      <c r="C15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>161</v>
-      </c>
-      <c r="C17" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>163</v>
-      </c>
-      <c r="C18" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>167</v>
-      </c>
-      <c r="C20" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C21" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3890,7 +3904,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3898,7 +3912,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3906,7 +3920,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3914,7 +3928,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3945,7 +3959,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3953,7 +3967,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3961,7 +3975,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3969,7 +3983,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3977,7 +3991,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -4004,28 +4018,28 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="C1" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="E1" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="G1" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="H1" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="I1" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4033,22 +4047,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
       <c r="E2" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>191</v>
+        <v>157</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
       <c r="H2" s="4">
         <v>45250</v>
@@ -4062,22 +4076,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>160</v>
       </c>
       <c r="E3" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="H3" s="4">
         <v>45231</v>
@@ -4107,10 +4121,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4186,10 +4200,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix DB and IMG data
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uithcm-my.sharepoint.com/personal/21520442_ms_uit_edu_vn/Documents/HKV/Internet &amp; Công nghệ web/FurnitureWebsite/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="547" documentId="14_{7FF668E4-114F-45F3-93BD-413DF14B2BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFD18C67-CF38-4B93-82A1-7B3DBED5C7B1}"/>
+  <xr:revisionPtr revIDLastSave="549" documentId="14_{7FF668E4-114F-45F3-93BD-413DF14B2BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AFE5214-5EC6-4BB0-8FB7-675DA7BE18AF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EDD4E223-FED4-45DA-A9CC-BEB910C23BCF}"/>
   </bookViews>
@@ -571,151 +571,151 @@
     <t>ImgDirect</t>
   </si>
   <si>
-    <t>\img\Products_Photos\1</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\2</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\3</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\4</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\5</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\6</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\7</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\8</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\9</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\10</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\11</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\12</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\13</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\14</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\15</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\16</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\17</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\18</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\19</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\20</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\21</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\22</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\23</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\24</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\25</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\26</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\27</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\28</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\29</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\30</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\31</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\32</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\33</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\34</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\35</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\36</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\37</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\38</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\39</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\40</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\41</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\42</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\43</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\44</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\45</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\46</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\47</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\48</t>
-  </si>
-  <si>
-    <t>\img\Products_Photos\49</t>
+    <t>\assets\Furniture_Photos\Products_Photos\P0001</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0002</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0003</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0004</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0005</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0006</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0007</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0008</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0009</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0010</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0011</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0012</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0013</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0014</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0015</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0016</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0017</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0018</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0019</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0020</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0021</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0022</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0023</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0024</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0025</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0026</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0027</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0028</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0029</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0030</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0031</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0032</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0033</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0034</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0035</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0036</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0037</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0038</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0039</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0040</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0041</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0042</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0043</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0044</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0045</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0046</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0047</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0048</t>
+  </si>
+  <si>
+    <t>\assets\Furniture_Photos\Products_Photos\P0049</t>
   </si>
 </sst>
 </file>
@@ -804,6 +804,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1105,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4AED73-D74A-4FB9-9481-FBDC8FFD72A2}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add sample for database
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,20 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uithcm-my.sharepoint.com/personal/21520442_ms_uit_edu_vn/Documents/HKV/Internet &amp; Công nghệ web/FurnitureWebsite/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="549" documentId="14_{7FF668E4-114F-45F3-93BD-413DF14B2BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AFE5214-5EC6-4BB0-8FB7-675DA7BE18AF}"/>
+  <xr:revisionPtr revIDLastSave="787" documentId="14_{7FF668E4-114F-45F3-93BD-413DF14B2BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{230AE1CB-7E9D-42A2-8051-34D26AB1CBE8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EDD4E223-FED4-45DA-A9CC-BEB910C23BCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="4" xr2:uid="{EDD4E223-FED4-45DA-A9CC-BEB910C23BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCTS" sheetId="2" r:id="rId1"/>
     <sheet name="TAGS" sheetId="1" r:id="rId2"/>
     <sheet name="PRODUCT_TAG" sheetId="3" r:id="rId3"/>
     <sheet name="COLOURS" sheetId="4" r:id="rId4"/>
-    <sheet name="PERMISSIONS" sheetId="5" r:id="rId5"/>
-    <sheet name="ROLES" sheetId="6" r:id="rId6"/>
-    <sheet name="USERS" sheetId="7" r:id="rId7"/>
-    <sheet name="ROLE_PERMISSION" sheetId="8" r:id="rId8"/>
-    <sheet name="USER_ROLE" sheetId="9" r:id="rId9"/>
+    <sheet name="VOUCHERS" sheetId="10" r:id="rId5"/>
+    <sheet name="PERMISSIONS" sheetId="5" r:id="rId6"/>
+    <sheet name="ROLES" sheetId="6" r:id="rId7"/>
+    <sheet name="USERS" sheetId="7" r:id="rId8"/>
+    <sheet name="RECEIPTS" sheetId="12" r:id="rId9"/>
+    <sheet name="ROLE_PERMISSION" sheetId="8" r:id="rId10"/>
+    <sheet name="USER_ROLE" sheetId="9" r:id="rId11"/>
+    <sheet name="RECEIPT_DETAIL" sheetId="13" r:id="rId12"/>
+    <sheet name="LIKE_PRODUCT" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="271">
   <si>
     <t>Bedroom</t>
   </si>
@@ -517,12 +521,6 @@
     <t>Hưng</t>
   </si>
   <si>
-    <t>0900445424</t>
-  </si>
-  <si>
-    <t>Hung@gmail.com</t>
-  </si>
-  <si>
     <t>tan</t>
   </si>
   <si>
@@ -538,9 +536,6 @@
     <t>0948582733</t>
   </si>
   <si>
-    <t>21520442@gm.uit.edu</t>
-  </si>
-  <si>
     <t>RoleID</t>
   </si>
   <si>
@@ -571,158 +566,308 @@
     <t>ImgDirect</t>
   </si>
   <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0001</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0002</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0003</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0004</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0005</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0006</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0007</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0008</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0009</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0010</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0011</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0012</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0013</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0014</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0015</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0016</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0017</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0018</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0019</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0020</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0021</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0022</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0023</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0024</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0025</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0026</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0027</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0028</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0029</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0030</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0031</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0032</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0033</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0034</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0035</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0036</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0037</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0038</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0039</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0040</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0041</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0042</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0043</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0044</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0045</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0046</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0047</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0048</t>
-  </si>
-  <si>
-    <t>\assets\Furniture_Photos\Products_Photos\P0049</t>
+    <t>/assets/Furniture_Photos/Products_Photos/P0001</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0002</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0003</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0004</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0005</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0006</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0007</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0008</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0009</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0010</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0011</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0012</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0013</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0014</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0015</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0016</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0017</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0018</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0019</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0020</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0021</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0022</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0023</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0024</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0025</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0026</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0027</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0028</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0029</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0030</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0031</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0032</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0033</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0034</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0035</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0036</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0037</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0038</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0039</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0040</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0041</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0042</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0043</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0044</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0045</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0046</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0047</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0048</t>
+  </si>
+  <si>
+    <t>/assets/Furniture_Photos/Products_Photos/P0049</t>
+  </si>
+  <si>
+    <t>21520895gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>21520442gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>21522093gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>21521247gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>21521214gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>21522596gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>21520949gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>Hoàng</t>
+  </si>
+  <si>
+    <t>Nguyễn Huy</t>
+  </si>
+  <si>
+    <t>Như</t>
+  </si>
+  <si>
+    <t>Trần Thị Tâm</t>
+  </si>
+  <si>
+    <t>Nhân</t>
+  </si>
+  <si>
+    <t>Đỗ Trọng</t>
+  </si>
+  <si>
+    <t>Thành</t>
+  </si>
+  <si>
+    <t>Lê Nam</t>
+  </si>
+  <si>
+    <t>Kha</t>
+  </si>
+  <si>
+    <t>Nguyễn Viết</t>
+  </si>
+  <si>
+    <t>0948582734</t>
+  </si>
+  <si>
+    <t>0948582735</t>
+  </si>
+  <si>
+    <t>0948582736</t>
+  </si>
+  <si>
+    <t>0948582737</t>
+  </si>
+  <si>
+    <t>0948582738</t>
+  </si>
+  <si>
+    <t>0948582732</t>
+  </si>
+  <si>
+    <t>hoang</t>
+  </si>
+  <si>
+    <t>nhu</t>
+  </si>
+  <si>
+    <t>nhan</t>
+  </si>
+  <si>
+    <t>thanh</t>
+  </si>
+  <si>
+    <t>kha</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>10% discount</t>
+  </si>
+  <si>
+    <t>1% discount</t>
+  </si>
+  <si>
+    <t>2% discount</t>
+  </si>
+  <si>
+    <t>5% discount</t>
+  </si>
+  <si>
+    <t>100$ discount</t>
+  </si>
+  <si>
+    <t>200$ discount</t>
+  </si>
+  <si>
+    <t>500$ discount</t>
+  </si>
+  <si>
+    <t>1000$ discount</t>
+  </si>
+  <si>
+    <t>2000$ discount</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ReceiptID</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>ColourID</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>ValidDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -742,21 +887,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -775,22 +905,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1109,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4AED73-D74A-4FB9-9481-FBDC8FFD72A2}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1153,7 +1278,7 @@
         <v>72</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1185,7 +1310,7 @@
         <v>60</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1217,7 +1342,7 @@
         <v>47</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1249,7 +1374,7 @@
         <v>40</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1260,7 +1385,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D5" s="1">
         <v>2475</v>
@@ -1281,7 +1406,7 @@
         <v>72</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1292,7 +1417,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D6" s="1">
         <v>1950</v>
@@ -1313,7 +1438,7 @@
         <v>50</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1345,7 +1470,7 @@
         <v>48</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1377,7 +1502,7 @@
         <v>82</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1409,7 +1534,7 @@
         <v>76</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1441,7 +1566,7 @@
         <v>50</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1473,7 +1598,7 @@
         <v>80</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1505,7 +1630,7 @@
         <v>75</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1537,7 +1662,7 @@
         <v>84</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1569,7 +1694,7 @@
         <v>25</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1601,7 +1726,7 @@
         <v>35</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1633,7 +1758,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1665,7 +1790,7 @@
         <v>15</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1697,7 +1822,7 @@
         <v>40</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1729,7 +1854,7 @@
         <v>30</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1761,7 +1886,7 @@
         <v>34</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1793,7 +1918,7 @@
         <v>42</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1825,7 +1950,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1857,7 +1982,7 @@
         <v>30</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1889,7 +2014,7 @@
         <v>40</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1921,7 +2046,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1953,7 +2078,7 @@
         <v>25</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1985,7 +2110,7 @@
         <v>30</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2017,7 +2142,7 @@
         <v>36</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2049,7 +2174,7 @@
         <v>30</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2081,7 +2206,7 @@
         <v>40</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2113,7 +2238,7 @@
         <v>19.5</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2124,7 +2249,7 @@
         <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D32" s="1">
         <v>2450</v>
@@ -2145,7 +2270,7 @@
         <v>96</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2177,7 +2302,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2188,7 +2313,7 @@
         <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D34" s="1">
         <v>755</v>
@@ -2209,7 +2334,7 @@
         <v>19.5</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2220,7 +2345,7 @@
         <v>46</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D35" s="1">
         <v>4275</v>
@@ -2241,7 +2366,7 @@
         <v>96</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2252,7 +2377,7 @@
         <v>47</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D36" s="1">
         <v>2925</v>
@@ -2273,7 +2398,7 @@
         <v>48</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2284,7 +2409,7 @@
         <v>48</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D37" s="1">
         <v>525</v>
@@ -2305,7 +2430,7 @@
         <v>29</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2337,7 +2462,7 @@
         <v>43</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2369,7 +2494,7 @@
         <v>100</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2380,7 +2505,7 @@
         <v>50</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D40" s="1">
         <v>4250</v>
@@ -2401,7 +2526,7 @@
         <v>100</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2433,7 +2558,7 @@
         <v>100</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2465,7 +2590,7 @@
         <v>100</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2497,7 +2622,7 @@
         <v>100</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2529,7 +2654,7 @@
         <v>100</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2561,7 +2686,7 @@
         <v>70</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2593,7 +2718,7 @@
         <v>75</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2625,7 +2750,7 @@
         <v>65</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2657,7 +2782,7 @@
         <v>100</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2689,7 +2814,7 @@
         <v>58</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2721,11 +2846,674 @@
         <v>100</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEA6A849-BFEE-400F-9008-E3C8B4D1FA2B}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB2E6EE-AEA3-4535-BE12-6131960589AD}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52E565C-EC24-4DF1-BA07-B63399142338}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>35</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>32</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DF7F399-5F35-45F3-AE72-32E992ABBF4F}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>268</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2858,14 +3646,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5D2C1-A73E-40E7-8792-6F2DAABC2E9D}">
   <dimension ref="A1:B119"/>
   <sheetViews>
-    <sheetView zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="1" max="2" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3831,7 +4618,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3886,11 +4673,199 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18B4DFD-6F94-403F-BE93-F73DB7D18FC8}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2">
+        <v>0.01</v>
+      </c>
+      <c r="E2" s="2">
+        <v>182988</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3">
+        <v>0.02</v>
+      </c>
+      <c r="E3" s="2">
+        <v>182988</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D4">
+        <v>0.05</v>
+      </c>
+      <c r="E4" s="2">
+        <v>182988</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>182988</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6" s="2">
+        <v>182988</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C7" t="s">
+        <v>250</v>
+      </c>
+      <c r="D7">
+        <v>200</v>
+      </c>
+      <c r="E7" s="2">
+        <v>182988</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D8">
+        <v>500</v>
+      </c>
+      <c r="E8" s="2">
+        <v>182988</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C9" t="s">
+        <v>250</v>
+      </c>
+      <c r="D9">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="2">
+        <v>182988</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>259</v>
+      </c>
+      <c r="C10" t="s">
+        <v>250</v>
+      </c>
+      <c r="D10">
+        <v>2000</v>
+      </c>
+      <c r="E10" s="2">
+        <v>182988</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622C4E1A-38EA-403C-8164-59B4013D23A7}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3940,12 +4915,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E4EE0F-4D09-4BAE-B55D-70C2134EA579}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3971,7 +4946,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3979,7 +4954,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3987,7 +4962,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3995,7 +4970,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -4003,18 +4978,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C7A6A2-00F5-4D6A-B4A1-0FD163EC6D74}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4033,7 +5014,7 @@
       <c r="E1" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>150</v>
       </c>
       <c r="G1" t="s">
@@ -4060,16 +5041,16 @@
         <v>156</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H2" s="4">
-        <v>45250</v>
+        <v>160</v>
+      </c>
+      <c r="F2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H2" s="2">
+        <v>45231</v>
       </c>
       <c r="I2">
         <v>2003</v>
@@ -4080,150 +5061,311 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" t="s">
         <v>159</v>
       </c>
-      <c r="C3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>161</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="H3" s="4">
-        <v>45231</v>
+      <c r="G3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H3" s="2">
+        <v>45232</v>
       </c>
       <c r="I3">
         <v>2003</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H4" s="2">
+        <v>45233</v>
+      </c>
+      <c r="I4">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G5" t="s">
+        <v>224</v>
+      </c>
+      <c r="H5" s="2">
+        <v>45234</v>
+      </c>
+      <c r="I5">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F6" t="s">
+        <v>240</v>
+      </c>
+      <c r="G6" t="s">
+        <v>225</v>
+      </c>
+      <c r="H6" s="2">
+        <v>45235</v>
+      </c>
+      <c r="I6">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D7" t="s">
+        <v>234</v>
+      </c>
+      <c r="E7" t="s">
+        <v>235</v>
+      </c>
+      <c r="F7" t="s">
+        <v>241</v>
+      </c>
+      <c r="G7" t="s">
+        <v>226</v>
+      </c>
+      <c r="H7" s="2">
+        <v>45236</v>
+      </c>
+      <c r="I7">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" t="s">
+        <v>237</v>
+      </c>
+      <c r="F8" t="s">
+        <v>242</v>
+      </c>
+      <c r="G8" t="s">
+        <v>227</v>
+      </c>
+      <c r="H8" s="2">
+        <v>45237</v>
+      </c>
+      <c r="I8">
+        <v>2003</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{38BDA040-D4FD-4998-BC66-4A91A676963A}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{D4BC4DF2-C5E5-4C67-88D5-598F4068CE44}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEA6A849-BFEE-400F-9008-E3C8B4D1FA2B}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB2E6EE-AEA3-4535-BE12-6131960589AD}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524D3CEE-44F0-40C8-9DD0-100D156A29DC}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>167</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="C1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <v>45261</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" s="2">
+        <v>45261</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45261</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45261</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45261</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45261</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix data and add sp
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uithcm-my.sharepoint.com/personal/21520442_ms_uit_edu_vn/Documents/HKV/Internet &amp; Công nghệ web/FurnitureWebsite/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="787" documentId="14_{7FF668E4-114F-45F3-93BD-413DF14B2BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{230AE1CB-7E9D-42A2-8051-34D26AB1CBE8}"/>
+  <xr:revisionPtr revIDLastSave="820" documentId="14_{7FF668E4-114F-45F3-93BD-413DF14B2BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B82CEFAC-E4C1-4BF9-83D9-3CF743EFAA74}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="4" xr2:uid="{EDD4E223-FED4-45DA-A9CC-BEB910C23BCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EDD4E223-FED4-45DA-A9CC-BEB910C23BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCTS" sheetId="2" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="USER_ROLE" sheetId="9" r:id="rId11"/>
     <sheet name="RECEIPT_DETAIL" sheetId="13" r:id="rId12"/>
     <sheet name="LIKE_PRODUCT" sheetId="15" r:id="rId13"/>
+    <sheet name="COMMENTS" sheetId="16" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="280">
   <si>
     <t>Bedroom</t>
   </si>
@@ -566,153 +567,6 @@
     <t>ImgDirect</t>
   </si>
   <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0001</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0002</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0003</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0004</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0005</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0006</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0007</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0008</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0009</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0010</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0011</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0012</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0013</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0014</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0015</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0016</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0017</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0018</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0019</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0020</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0021</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0022</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0023</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0024</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0025</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0026</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0027</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0028</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0029</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0030</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0031</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0032</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0033</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0034</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0035</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0036</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0037</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0038</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0039</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0040</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0041</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0042</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0043</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0044</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0045</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0046</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0047</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0048</t>
-  </si>
-  <si>
-    <t>/assets/Furniture_Photos/Products_Photos/P0049</t>
-  </si>
-  <si>
     <t>21520895gm.uit.edu.vn</t>
   </si>
   <si>
@@ -861,6 +715,180 @@
   </si>
   <si>
     <t>ValidDate</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Ở</t>
+  </si>
+  <si>
+    <t>đâu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cơ </t>
+  </si>
+  <si>
+    <t>tôi</t>
+  </si>
+  <si>
+    <t>cũng</t>
+  </si>
+  <si>
+    <t>không</t>
+  </si>
+  <si>
+    <t>biết</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0001</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0002</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0003</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0004</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0005</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0006</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0007</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0008</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0009</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0010</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0011</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0012</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0013</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0014</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0015</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0016</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0017</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0018</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0019</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0020</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0021</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0022</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0023</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0024</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0025</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0026</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0027</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0028</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0029</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0030</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0031</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0032</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0033</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0034</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0035</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0036</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0037</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0038</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0039</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0040</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0041</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0042</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0043</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0044</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0045</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0046</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0047</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0048</t>
+  </si>
+  <si>
+    <t>../assets/Furniture_Photos/Products_Photos/P0049</t>
   </si>
 </sst>
 </file>
@@ -1234,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4AED73-D74A-4FB9-9481-FBDC8FFD72A2}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1310,7 +1338,7 @@
         <v>60</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>172</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1342,7 +1370,7 @@
         <v>47</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>173</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1374,7 +1402,7 @@
         <v>40</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>174</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1406,7 +1434,7 @@
         <v>72</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>175</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1438,7 +1466,7 @@
         <v>50</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>176</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1470,7 +1498,7 @@
         <v>48</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>177</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1502,7 +1530,7 @@
         <v>82</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>178</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1534,7 +1562,7 @@
         <v>76</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>179</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1566,7 +1594,7 @@
         <v>50</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1598,7 +1626,7 @@
         <v>80</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>181</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1630,7 +1658,7 @@
         <v>75</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>182</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1662,7 +1690,7 @@
         <v>84</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>183</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1694,7 +1722,7 @@
         <v>25</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>184</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1726,7 +1754,7 @@
         <v>35</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>185</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1758,7 +1786,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>186</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1790,7 +1818,7 @@
         <v>15</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>187</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1822,7 +1850,7 @@
         <v>40</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1854,7 +1882,7 @@
         <v>30</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>189</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1886,7 +1914,7 @@
         <v>34</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>190</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1918,7 +1946,7 @@
         <v>42</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>191</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1950,7 +1978,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>192</v>
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1982,7 +2010,7 @@
         <v>30</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>193</v>
+        <v>252</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2014,7 +2042,7 @@
         <v>40</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>194</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -2046,7 +2074,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>195</v>
+        <v>254</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2078,7 +2106,7 @@
         <v>25</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>196</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2110,7 +2138,7 @@
         <v>30</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>197</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2142,7 +2170,7 @@
         <v>36</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>198</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2174,7 +2202,7 @@
         <v>30</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>199</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2206,7 +2234,7 @@
         <v>40</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>200</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2238,7 +2266,7 @@
         <v>19.5</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>201</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2270,7 +2298,7 @@
         <v>96</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>202</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2302,7 +2330,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>203</v>
+        <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2334,7 +2362,7 @@
         <v>19.5</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>204</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2366,7 +2394,7 @@
         <v>96</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>205</v>
+        <v>264</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2398,7 +2426,7 @@
         <v>48</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>206</v>
+        <v>265</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2430,7 +2458,7 @@
         <v>29</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>207</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2462,7 +2490,7 @@
         <v>43</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>208</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2494,7 +2522,7 @@
         <v>100</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>209</v>
+        <v>268</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2526,7 +2554,7 @@
         <v>100</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>210</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2558,7 +2586,7 @@
         <v>100</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>211</v>
+        <v>270</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2590,7 +2618,7 @@
         <v>100</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>212</v>
+        <v>271</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2622,7 +2650,7 @@
         <v>100</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>213</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2654,7 +2682,7 @@
         <v>100</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>214</v>
+        <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2686,7 +2714,7 @@
         <v>70</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>215</v>
+        <v>274</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2718,7 +2746,7 @@
         <v>75</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>216</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2750,7 +2778,7 @@
         <v>65</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>217</v>
+        <v>276</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2782,7 +2810,7 @@
         <v>100</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>218</v>
+        <v>277</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2814,7 +2842,7 @@
         <v>58</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>219</v>
+        <v>278</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2846,7 +2874,7 @@
         <v>100</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>220</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -3025,16 +3053,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>264</v>
+        <v>215</v>
       </c>
       <c r="B1" t="s">
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>265</v>
+        <v>216</v>
       </c>
       <c r="D1" t="s">
-        <v>266</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3299,7 +3327,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3312,7 +3340,7 @@
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>267</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3323,7 +3351,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3334,7 +3362,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3345,7 +3373,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3356,7 +3384,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3367,7 +3395,7 @@
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3378,7 +3406,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3389,7 +3417,7 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3400,7 +3428,7 @@
         <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3411,7 +3439,7 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3422,7 +3450,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3433,7 +3461,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3444,7 +3472,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3455,7 +3483,7 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3466,7 +3494,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3477,7 +3505,7 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3488,7 +3516,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3499,7 +3527,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3510,7 +3538,288 @@
         <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>268</v>
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B9B834E-0D6D-4D92-9524-92BEA70914DD}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D9">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>219</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>219</v>
+      </c>
+      <c r="D11">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>219</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>219</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>219</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D16">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>219</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>219</v>
+      </c>
+      <c r="D18">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>219</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4676,7 +4985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18B4DFD-6F94-403F-BE93-F73DB7D18FC8}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -4693,13 +5002,13 @@
         <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>249</v>
+        <v>200</v>
       </c>
       <c r="D1" t="s">
-        <v>250</v>
+        <v>201</v>
       </c>
       <c r="E1" t="s">
-        <v>270</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4707,10 +5016,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>252</v>
+        <v>203</v>
       </c>
       <c r="C2" t="s">
-        <v>260</v>
+        <v>211</v>
       </c>
       <c r="D2">
         <v>0.01</v>
@@ -4724,10 +5033,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>260</v>
+        <v>211</v>
       </c>
       <c r="D3">
         <v>0.02</v>
@@ -4741,10 +5050,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>254</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>260</v>
+        <v>211</v>
       </c>
       <c r="D4">
         <v>0.05</v>
@@ -4758,10 +5067,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>251</v>
+        <v>202</v>
       </c>
       <c r="C5" t="s">
-        <v>260</v>
+        <v>211</v>
       </c>
       <c r="D5">
         <v>0.1</v>
@@ -4775,10 +5084,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="C6" t="s">
-        <v>250</v>
+        <v>201</v>
       </c>
       <c r="D6">
         <v>100</v>
@@ -4792,10 +5101,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="C7" t="s">
-        <v>250</v>
+        <v>201</v>
       </c>
       <c r="D7">
         <v>200</v>
@@ -4809,10 +5118,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="C8" t="s">
-        <v>250</v>
+        <v>201</v>
       </c>
       <c r="D8">
         <v>500</v>
@@ -4826,10 +5135,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>258</v>
+        <v>209</v>
       </c>
       <c r="C9" t="s">
-        <v>250</v>
+        <v>201</v>
       </c>
       <c r="D9">
         <v>1000</v>
@@ -4843,10 +5152,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>259</v>
+        <v>210</v>
       </c>
       <c r="C10" t="s">
-        <v>250</v>
+        <v>201</v>
       </c>
       <c r="D10">
         <v>2000</v>
@@ -4980,10 +5289,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C7A6A2-00F5-4D6A-B4A1-0FD163EC6D74}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4993,12 +5302,13 @@
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -5015,19 +5325,22 @@
         <v>149</v>
       </c>
       <c r="F1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" t="s">
         <v>150</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>151</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>152</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5044,19 +5357,22 @@
         <v>160</v>
       </c>
       <c r="F2" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="G2" t="s">
-        <v>221</v>
-      </c>
-      <c r="H2" s="2">
+        <v>194</v>
+      </c>
+      <c r="H2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I2" s="2">
         <v>45231</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>2003</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5073,160 +5389,178 @@
         <v>159</v>
       </c>
       <c r="F3" t="s">
+        <v>224</v>
+      </c>
+      <c r="G3" t="s">
         <v>161</v>
       </c>
-      <c r="G3" t="s">
-        <v>222</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="H3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I3" s="2">
         <v>45232</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>2003</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>244</v>
+        <v>195</v>
       </c>
       <c r="C4" t="s">
-        <v>244</v>
+        <v>195</v>
       </c>
       <c r="D4" t="s">
-        <v>228</v>
+        <v>179</v>
       </c>
       <c r="E4" t="s">
-        <v>229</v>
+        <v>180</v>
       </c>
       <c r="F4" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="G4" t="s">
-        <v>223</v>
-      </c>
-      <c r="H4" s="2">
+        <v>189</v>
+      </c>
+      <c r="H4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I4" s="2">
         <v>45233</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2003</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>245</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>245</v>
+        <v>196</v>
       </c>
       <c r="D5" t="s">
-        <v>230</v>
+        <v>181</v>
       </c>
       <c r="E5" t="s">
-        <v>231</v>
+        <v>182</v>
       </c>
       <c r="F5" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="G5" t="s">
-        <v>224</v>
-      </c>
-      <c r="H5" s="2">
+        <v>190</v>
+      </c>
+      <c r="H5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I5" s="2">
         <v>45234</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>2003</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>197</v>
       </c>
       <c r="C6" t="s">
-        <v>246</v>
+        <v>197</v>
       </c>
       <c r="D6" t="s">
-        <v>232</v>
+        <v>183</v>
       </c>
       <c r="E6" t="s">
-        <v>233</v>
+        <v>184</v>
       </c>
       <c r="F6" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="G6" t="s">
-        <v>225</v>
-      </c>
-      <c r="H6" s="2">
+        <v>191</v>
+      </c>
+      <c r="H6" t="s">
+        <v>176</v>
+      </c>
+      <c r="I6" s="2">
         <v>45235</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>2003</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>247</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
-        <v>247</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
-        <v>234</v>
+        <v>185</v>
       </c>
       <c r="E7" t="s">
-        <v>235</v>
+        <v>186</v>
       </c>
       <c r="F7" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="G7" t="s">
-        <v>226</v>
-      </c>
-      <c r="H7" s="2">
+        <v>192</v>
+      </c>
+      <c r="H7" t="s">
+        <v>177</v>
+      </c>
+      <c r="I7" s="2">
         <v>45236</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>2003</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="C8" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="D8" t="s">
-        <v>236</v>
+        <v>187</v>
       </c>
       <c r="E8" t="s">
-        <v>237</v>
+        <v>188</v>
       </c>
       <c r="F8" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="G8" t="s">
-        <v>227</v>
-      </c>
-      <c r="H8" s="2">
+        <v>193</v>
+      </c>
+      <c r="H8" t="s">
+        <v>178</v>
+      </c>
+      <c r="I8" s="2">
         <v>45237</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>2003</v>
       </c>
     </row>
@@ -5254,16 +5588,16 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>261</v>
+        <v>212</v>
       </c>
       <c r="C1" t="s">
-        <v>262</v>
+        <v>213</v>
       </c>
       <c r="D1" t="s">
         <v>164</v>
       </c>
       <c r="E1" t="s">
-        <v>263</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5280,7 +5614,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>269</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5297,7 +5631,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>269</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -5314,7 +5648,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>269</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5331,7 +5665,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>269</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -5348,7 +5682,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>269</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -5365,7 +5699,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>269</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove diacritic in db
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uithcm-my.sharepoint.com/personal/21520442_ms_uit_edu_vn/Documents/HKV/Internet &amp; Công nghệ web/FurnitureWebsite/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="820" documentId="14_{7FF668E4-114F-45F3-93BD-413DF14B2BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B82CEFAC-E4C1-4BF9-83D9-3CF743EFAA74}"/>
+  <xr:revisionPtr revIDLastSave="889" documentId="14_{7FF668E4-114F-45F3-93BD-413DF14B2BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40375B41-A147-45C1-A3F1-FCE64A0AE2F7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EDD4E223-FED4-45DA-A9CC-BEB910C23BCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="7" activeTab="7" xr2:uid="{EDD4E223-FED4-45DA-A9CC-BEB910C23BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCTS" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="286">
   <si>
     <t>Bedroom</t>
   </si>
@@ -516,24 +516,9 @@
     <t>admin</t>
   </si>
   <si>
-    <t>hehehe</t>
-  </si>
-  <si>
-    <t>Hưng</t>
-  </si>
-  <si>
     <t>tan</t>
   </si>
   <si>
-    <t>Tân</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Đặng Huỳnh Vĩnh </t>
-  </si>
-  <si>
-    <t>Nguyễn Hoàng</t>
-  </si>
-  <si>
     <t>0948582733</t>
   </si>
   <si>
@@ -588,36 +573,9 @@
     <t>21520949gm.uit.edu.vn</t>
   </si>
   <si>
-    <t>Hoàng</t>
-  </si>
-  <si>
-    <t>Nguyễn Huy</t>
-  </si>
-  <si>
-    <t>Như</t>
-  </si>
-  <si>
-    <t>Trần Thị Tâm</t>
-  </si>
-  <si>
-    <t>Nhân</t>
-  </si>
-  <si>
-    <t>Đỗ Trọng</t>
-  </si>
-  <si>
-    <t>Thành</t>
-  </si>
-  <si>
-    <t>Lê Nam</t>
-  </si>
-  <si>
     <t>Kha</t>
   </si>
   <si>
-    <t>Nguyễn Viết</t>
-  </si>
-  <si>
     <t>0948582734</t>
   </si>
   <si>
@@ -720,27 +678,6 @@
     <t>Address</t>
   </si>
   <si>
-    <t>Ở</t>
-  </si>
-  <si>
-    <t>đâu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cơ </t>
-  </si>
-  <si>
-    <t>tôi</t>
-  </si>
-  <si>
-    <t>cũng</t>
-  </si>
-  <si>
-    <t>không</t>
-  </si>
-  <si>
-    <t>biết</t>
-  </si>
-  <si>
     <t>Rating</t>
   </si>
   <si>
@@ -889,6 +826,87 @@
   </si>
   <si>
     <t>../assets/Furniture_Photos/Products_Photos/P0049</t>
+  </si>
+  <si>
+    <t>Ehehehe1</t>
+  </si>
+  <si>
+    <t>Tan31123</t>
+  </si>
+  <si>
+    <t>HuyHoang1</t>
+  </si>
+  <si>
+    <t>TamNhu12</t>
+  </si>
+  <si>
+    <t>TrongNhan1</t>
+  </si>
+  <si>
+    <t>NamThanh1</t>
+  </si>
+  <si>
+    <t>VietKha1</t>
+  </si>
+  <si>
+    <t>Hung</t>
+  </si>
+  <si>
+    <t>Nguyen Hoang</t>
+  </si>
+  <si>
+    <t>Duong Han Thuyen, khu pho 6 P, Thu Duc, Thanh pho Ho Chi Minh</t>
+  </si>
+  <si>
+    <t>Tan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dang Huynh Vinh </t>
+  </si>
+  <si>
+    <t>6 Duong so 447, Tang Nhon Phu A, Thu Duc, Thanh pho Ho Chi Minh</t>
+  </si>
+  <si>
+    <t>Hoang</t>
+  </si>
+  <si>
+    <t>Nguyen Huy</t>
+  </si>
+  <si>
+    <t>VRG2+9GJ, D. Quang Truong Sang Tao, Dong Hoa, Di An, Binh Duong</t>
+  </si>
+  <si>
+    <t>Nhu</t>
+  </si>
+  <si>
+    <t>Tran Thi Tam</t>
+  </si>
+  <si>
+    <t>VRJ5+JHP, Duong Ta Quang Buu, Dong Hoa, Di An, Binh Duong</t>
+  </si>
+  <si>
+    <t>Nhan</t>
+  </si>
+  <si>
+    <t>Do Trong</t>
+  </si>
+  <si>
+    <t>D. Mac Dinh Chi, Khu pho Tan Hoa, Di An, Binh Duong</t>
+  </si>
+  <si>
+    <t>Thanh</t>
+  </si>
+  <si>
+    <t>Le Nam</t>
+  </si>
+  <si>
+    <t>Phuong Ben Thanh, Quan 1, Thanh pho Ho Chi Minh</t>
+  </si>
+  <si>
+    <t>Nguyen Viet</t>
+  </si>
+  <si>
+    <t>01 Cong xa Paris, Ben Nghe, Quan 1, Thanh pho Ho Chi Minh</t>
   </si>
 </sst>
 </file>
@@ -936,12 +954,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1262,7 +1282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4AED73-D74A-4FB9-9481-FBDC8FFD72A2}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
@@ -1306,7 +1326,7 @@
         <v>72</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1338,7 +1358,7 @@
         <v>60</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1370,7 +1390,7 @@
         <v>47</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1402,7 +1422,7 @@
         <v>40</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1413,7 +1433,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D5" s="1">
         <v>2475</v>
@@ -1434,7 +1454,7 @@
         <v>72</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1445,7 +1465,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D6" s="1">
         <v>1950</v>
@@ -1466,7 +1486,7 @@
         <v>50</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1498,7 +1518,7 @@
         <v>48</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1530,7 +1550,7 @@
         <v>82</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1562,7 +1582,7 @@
         <v>76</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1594,7 +1614,7 @@
         <v>50</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1626,7 +1646,7 @@
         <v>80</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1658,7 +1678,7 @@
         <v>75</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1690,7 +1710,7 @@
         <v>84</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1722,7 +1742,7 @@
         <v>25</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1754,7 +1774,7 @@
         <v>35</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1786,7 +1806,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1818,7 +1838,7 @@
         <v>15</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1850,7 +1870,7 @@
         <v>40</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1882,7 +1902,7 @@
         <v>30</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1914,7 +1934,7 @@
         <v>34</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1946,7 +1966,7 @@
         <v>42</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1978,7 +1998,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2010,7 +2030,7 @@
         <v>30</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2042,7 +2062,7 @@
         <v>40</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -2074,7 +2094,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2106,7 +2126,7 @@
         <v>25</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2138,7 +2158,7 @@
         <v>30</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2170,7 +2190,7 @@
         <v>36</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2202,7 +2222,7 @@
         <v>30</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2234,7 +2254,7 @@
         <v>40</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2266,7 +2286,7 @@
         <v>19.5</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2277,7 +2297,7 @@
         <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D32" s="1">
         <v>2450</v>
@@ -2298,7 +2318,7 @@
         <v>96</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2330,7 +2350,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2341,7 +2361,7 @@
         <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D34" s="1">
         <v>755</v>
@@ -2362,7 +2382,7 @@
         <v>19.5</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2373,7 +2393,7 @@
         <v>46</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D35" s="1">
         <v>4275</v>
@@ -2394,7 +2414,7 @@
         <v>96</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2405,7 +2425,7 @@
         <v>47</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D36" s="1">
         <v>2925</v>
@@ -2426,7 +2446,7 @@
         <v>48</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2437,7 +2457,7 @@
         <v>48</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D37" s="1">
         <v>525</v>
@@ -2458,7 +2478,7 @@
         <v>29</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2490,7 +2510,7 @@
         <v>43</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2522,7 +2542,7 @@
         <v>100</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2533,7 +2553,7 @@
         <v>50</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D40" s="1">
         <v>4250</v>
@@ -2554,7 +2574,7 @@
         <v>100</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2586,7 +2606,7 @@
         <v>100</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2618,7 +2638,7 @@
         <v>100</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2650,7 +2670,7 @@
         <v>100</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2682,7 +2702,7 @@
         <v>100</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2714,7 +2734,7 @@
         <v>70</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2746,7 +2766,7 @@
         <v>75</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2778,7 +2798,7 @@
         <v>65</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2810,7 +2830,7 @@
         <v>100</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2842,7 +2862,7 @@
         <v>58</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2874,7 +2894,7 @@
         <v>100</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2895,10 +2915,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2974,10 +2994,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3053,16 +3073,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="B1" t="s">
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="D1" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3334,13 +3354,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B1" t="s">
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3351,7 +3371,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3362,7 +3382,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3373,7 +3393,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3384,7 +3404,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3395,7 +3415,7 @@
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3406,7 +3426,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3417,7 +3437,7 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3428,7 +3448,7 @@
         <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3439,7 +3459,7 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3450,7 +3470,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3461,7 +3481,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3472,7 +3492,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3483,7 +3503,7 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3494,7 +3514,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3505,7 +3525,7 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3516,7 +3536,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3527,7 +3547,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3538,7 +3558,7 @@
         <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3551,23 +3571,23 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B1" t="s">
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="D1" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3578,7 +3598,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3592,7 +3612,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D3">
         <v>0.5</v>
@@ -3606,7 +3626,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -3620,7 +3640,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D5">
         <v>1.5</v>
@@ -3634,7 +3654,7 @@
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -3648,7 +3668,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D7">
         <v>2.5</v>
@@ -3662,7 +3682,7 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -3676,7 +3696,7 @@
         <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D9">
         <v>3.5</v>
@@ -3690,7 +3710,7 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -3704,7 +3724,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D11">
         <v>4.5</v>
@@ -3718,7 +3738,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -3732,7 +3752,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -3746,7 +3766,7 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D14">
         <v>0.5</v>
@@ -3760,7 +3780,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3774,7 +3794,7 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D16">
         <v>1.5</v>
@@ -3788,7 +3808,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -3802,7 +3822,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D18">
         <v>2.5</v>
@@ -3816,7 +3836,7 @@
         <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -5002,13 +5022,13 @@
         <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="D1" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="E1" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5016,10 +5036,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="D2">
         <v>0.01</v>
@@ -5033,10 +5053,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="D3">
         <v>0.02</v>
@@ -5050,10 +5070,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="C4" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="D4">
         <v>0.05</v>
@@ -5067,10 +5087,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="D5">
         <v>0.1</v>
@@ -5084,10 +5104,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="C6" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D6">
         <v>100</v>
@@ -5101,10 +5121,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C7" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D7">
         <v>200</v>
@@ -5118,10 +5138,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="C8" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D8">
         <v>500</v>
@@ -5135,10 +5155,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="C9" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D9">
         <v>1000</v>
@@ -5152,10 +5172,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="C10" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D10">
         <v>2000</v>
@@ -5289,9 +5309,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C7A6A2-00F5-4D6A-B4A1-0FD163EC6D74}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -5303,12 +5323,12 @@
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -5325,7 +5345,7 @@
         <v>149</v>
       </c>
       <c r="F1" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="G1" t="s">
         <v>150</v>
@@ -5339,8 +5359,9 @@
       <c r="J1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S1" s="4"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5348,22 +5369,22 @@
         <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>259</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>266</v>
       </c>
       <c r="E2" t="s">
-        <v>160</v>
+        <v>267</v>
       </c>
       <c r="F2" t="s">
-        <v>223</v>
-      </c>
-      <c r="G2" t="s">
-        <v>194</v>
+        <v>268</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="H2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I2" s="2">
         <v>45231</v>
@@ -5371,31 +5392,32 @@
       <c r="J2">
         <v>2003</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>260</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>269</v>
       </c>
       <c r="E3" t="s">
-        <v>159</v>
+        <v>270</v>
       </c>
       <c r="F3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G3" t="s">
-        <v>161</v>
+        <v>271</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="H3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I3" s="2">
         <v>45232</v>
@@ -5403,31 +5425,32 @@
       <c r="J3">
         <v>2003</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>195</v>
+        <v>261</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>272</v>
       </c>
       <c r="E4" t="s">
-        <v>180</v>
+        <v>273</v>
       </c>
       <c r="F4" t="s">
-        <v>225</v>
-      </c>
-      <c r="G4" t="s">
-        <v>189</v>
+        <v>274</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="H4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I4" s="2">
         <v>45233</v>
@@ -5435,31 +5458,32 @@
       <c r="J4">
         <v>2003</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="C5" t="s">
-        <v>196</v>
+        <v>262</v>
       </c>
       <c r="D5" t="s">
-        <v>181</v>
+        <v>275</v>
       </c>
       <c r="E5" t="s">
-        <v>182</v>
+        <v>276</v>
       </c>
       <c r="F5" t="s">
-        <v>226</v>
-      </c>
-      <c r="G5" t="s">
-        <v>190</v>
+        <v>277</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="H5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I5" s="2">
         <v>45234</v>
@@ -5467,31 +5491,32 @@
       <c r="J5">
         <v>2003</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S5" s="4"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
-        <v>197</v>
+        <v>263</v>
       </c>
       <c r="D6" t="s">
-        <v>183</v>
+        <v>278</v>
       </c>
       <c r="E6" t="s">
-        <v>184</v>
+        <v>279</v>
       </c>
       <c r="F6" t="s">
-        <v>227</v>
-      </c>
-      <c r="G6" t="s">
-        <v>191</v>
+        <v>280</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="H6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I6" s="2">
         <v>45235</v>
@@ -5499,31 +5524,32 @@
       <c r="J6">
         <v>2003</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="C7" t="s">
-        <v>198</v>
+        <v>264</v>
       </c>
       <c r="D7" t="s">
-        <v>185</v>
+        <v>281</v>
       </c>
       <c r="E7" t="s">
-        <v>186</v>
+        <v>282</v>
       </c>
       <c r="F7" t="s">
-        <v>228</v>
-      </c>
-      <c r="G7" t="s">
-        <v>192</v>
+        <v>283</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="H7" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="I7" s="2">
         <v>45236</v>
@@ -5531,31 +5557,32 @@
       <c r="J7">
         <v>2003</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S7" s="4"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s">
-        <v>199</v>
+        <v>265</v>
       </c>
       <c r="D8" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="E8" t="s">
-        <v>188</v>
+        <v>284</v>
       </c>
       <c r="F8" t="s">
-        <v>229</v>
-      </c>
-      <c r="G8" t="s">
-        <v>193</v>
+        <v>285</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="H8" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="I8" s="2">
         <v>45237</v>
@@ -5588,16 +5615,16 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="C1" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E1" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5614,7 +5641,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5631,7 +5658,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -5648,7 +5675,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5665,7 +5692,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -5682,7 +5709,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -5699,7 +5726,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>